<commit_message>
min_results_per_frame.json contain correct last frame before exit
</commit_message>
<xml_diff>
--- a/results/ch2_permation_residue_comb.xlsx
+++ b/results/ch2_permation_residue_comb.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,14 +471,14 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>3631</t>
+          <t>3630</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>455</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -486,19 +486,19 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>455</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>3667</t>
+          <t>3666</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1073, 1105</t>
+          <t>780, 1073</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,12 +506,12 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1105</t>
+          <t>780</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>5131</t>
+          <t>5130</t>
         </is>
       </c>
     </row>
@@ -531,47 +531,47 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>4416</t>
+          <t>4415</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>130, 423, 1073</t>
+          <t>780, 1073, 1105</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>130, 130</t>
+          <t>1105</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>4995, 5330</t>
+          <t>4994</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>130, 130, 1073</t>
+          <t>130, 455, 780</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>130, 130</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>5270</t>
+          <t>5269, 6424</t>
         </is>
       </c>
     </row>
@@ -591,7 +591,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>5400</t>
+          <t>5399</t>
         </is>
       </c>
     </row>
@@ -602,83 +602,83 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>780, 780</t>
+          <t>780</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>5678, 5887</t>
+          <t>5677</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>130, 423, 1105</t>
+          <t>423, 1073, 1105</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>1105, 1105</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>5434</t>
+          <t>5329, 5433</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>98, 130, 748, 780, 1073</t>
+          <t>130, 423, 748, 1073</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>130, 130</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>6017</t>
+          <t>5886, 6561</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>98, 130, 748, 1073</t>
+          <t>98, 130, 748, 780, 1073</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>130, 130</t>
+          <t>130</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>5582, 6488</t>
+          <t>6016</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>130, 423, 748, 1073, SF</t>
+          <t>423, 748, 1073, 1105</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -686,19 +686,19 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>1105</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>6203</t>
+          <t>5581</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>130, 423, SF</t>
+          <t>423, 748, 780, 1073, SF</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -706,19 +706,19 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>780</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>6425</t>
+          <t>6202</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>130, 423, 780, 1073</t>
+          <t>130, 780, 1073, SF</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -726,19 +726,19 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>SF</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>6562</t>
+          <t>6487</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>98, 130, 780, 1073</t>
+          <t>130, 780, 1073, 1105</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -746,39 +746,39 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>1105</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>6360</t>
+          <t>6359</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>98, 130, 423, 780, 1105</t>
+          <t>98, 423, 780, 1073</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1105</t>
+          <t>1073, 98, 780, 423</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>6728</t>
+          <t>6798, 6798, 6798, 6798</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>98, 423, 780, 1073</t>
+          <t>98, 130, 130, 423, 780</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -786,19 +786,19 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>780</t>
+          <t>130</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>6671</t>
+          <t>6727</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>98, 98, 130, 455</t>
+          <t>98, 130, 423, 1073</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -811,7 +811,27 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>6749</t>
+          <t>6670</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>98, 130, 455, 780</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>780</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>6748</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
add offset (ion radius) to channels limits
</commit_message>
<xml_diff>
--- a/results/ch2_permation_residue_comb.xlsx
+++ b/results/ch2_permation_residue_comb.xlsx
@@ -471,7 +471,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>3630</t>
+          <t>3631</t>
         </is>
       </c>
     </row>
@@ -498,7 +498,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>780, 1073</t>
+          <t>1073, 1105</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,12 +506,12 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>780</t>
+          <t>1105</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>5130</t>
+          <t>5131</t>
         </is>
       </c>
     </row>
@@ -602,56 +602,56 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>780</t>
+          <t>780, 780</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>5677</t>
+          <t>5677, 5887</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>423, 1073, 1105</t>
+          <t>423, 1105, 1105</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1105, 1105</t>
+          <t>1105</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>5329, 5433</t>
+          <t>5331</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>130, 423, 748, 1073</t>
+          <t>423, 1073, 1105</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>130, 130</t>
+          <t>1105</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>5886, 6561</t>
+          <t>5433</t>
         </is>
       </c>
     </row>
@@ -678,20 +678,20 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>423, 748, 1073, 1105</t>
+          <t>98, 130, 748, 1073</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>1105</t>
+          <t>130, 130</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>5581</t>
+          <t>5582, 6488</t>
         </is>
       </c>
     </row>
@@ -718,7 +718,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>130, 780, 1073, SF</t>
+          <t>130, 423, 748, 1073</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -726,12 +726,12 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>SF</t>
+          <t>130</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>6487</t>
+          <t>6561</t>
         </is>
       </c>
     </row>
@@ -758,20 +758,20 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>98, 423, 780, 1073</t>
+          <t>98, 780, 1073</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1073, 98, 780, 423</t>
+          <t>1073, 98, 780</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>6798, 6798, 6798, 6798</t>
+          <t>6798, 6798, 6798</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
exclude ions that don not pemeate
</commit_message>
<xml_diff>
--- a/results/ch2_permation_residue_comb.xlsx
+++ b/results/ch2_permation_residue_comb.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -758,27 +758,27 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>98, 780, 1073</t>
+          <t>98, 130, 130, 423, 780</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1073, 98, 780</t>
+          <t>130</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>6798, 6798, 6798</t>
+          <t>6727</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>98, 130, 130, 423, 780</t>
+          <t>98, 130, 423, 1073</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -791,14 +791,14 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>6727</t>
+          <t>6670</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>98, 130, 423, 1073</t>
+          <t>98, 130, 455, 780</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -806,30 +806,10 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>780</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
-        <is>
-          <t>6670</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>98, 130, 455, 780</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>1</v>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>780</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
         <is>
           <t>6748</t>
         </is>

</xml_diff>

<commit_message>
Total forces added-segmanetaion fault
</commit_message>
<xml_diff>
--- a/results/ch2_permation_residue_comb.xlsx
+++ b/results/ch2_permation_residue_comb.xlsx
@@ -1,66 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Residue Combination</t>
-  </si>
-  <si>
-    <t>Count</t>
-  </si>
-  <si>
-    <t>Permeated Residues</t>
-  </si>
-  <si>
-    <t>Frames</t>
-  </si>
-  <si>
-    <t>423, 1105, 1105</t>
-  </si>
-  <si>
-    <t>1105</t>
-  </si>
-  <si>
-    <t>5331</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -75,35 +46,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -391,42 +420,62 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Residue Combination</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Permeated Residues</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Frames</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>423, 1105, 1105</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>1105</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>5331</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Total Forces fixed - calculated by openmm
</commit_message>
<xml_diff>
--- a/results/ch2_permation_residue_comb.xlsx
+++ b/results/ch2_permation_residue_comb.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>423, 1105, 1105</t>
+          <t>130, 455, 780</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -466,12 +466,132 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>5269</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>1073, 1105</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>1105</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>5131</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>130, 1073, 1105</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>1105</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>5399</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>423, 748, 780, 1073</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>780, 780</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>5677, 5887</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>423, 1105, 1105</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>1105</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
         <is>
           <t>5331</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>423, 1073, 1105</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>1105</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>5433</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>98, 130, 748, 1073</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>5582</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Ionic forces for all frames added
</commit_message>
<xml_diff>
--- a/results/ch2_permation_residue_comb.xlsx
+++ b/results/ch2_permation_residue_comb.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>130, 455, 780</t>
+          <t>130, 780</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -471,14 +471,14 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>5269</t>
+          <t>3631</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1073, 1105</t>
+          <t>455</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -486,19 +486,19 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>1105</t>
+          <t>455</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>5131</t>
+          <t>3666</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>130, 1073, 1105</t>
+          <t>1073, 1105</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -511,34 +511,34 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>5399</t>
+          <t>5131</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>423, 748, 780, 1073</t>
+          <t>130, 1073</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>780, 780</t>
+          <t>130</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>5677, 5887</t>
+          <t>4415</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>423, 1105, 1105</t>
+          <t>780, 1073, 1105</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -551,47 +551,267 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>5331</t>
+          <t>4994</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>423, 1073, 1105</t>
+          <t>130, 455, 780</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1105</t>
+          <t>130, 130</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>5433</t>
+          <t>5269, 6424</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>130, 1073, 1105</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>1105</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>5399</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>423, 748, 780, 1073</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>780, 780</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>5677, 5887</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>423, 1105, 1105</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>1105</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>5331</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>423, 1073, 1105</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1105</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>5433</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>98, 130, 748, 780, 1073</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>6016</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
           <t>98, 130, 748, 1073</t>
         </is>
       </c>
-      <c r="B8" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" t="inlineStr">
+      <c r="B13" t="n">
+        <v>2</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>130, 130</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>5582, 6488</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>423, 748, 780, 1073, SF</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>780</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>6202</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>130, 423, 748, 1073</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" t="inlineStr">
         <is>
           <t>130</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>5582</t>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>6561</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>130, 780, 1073, 1105</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>1105</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>6359</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>98, 130, 130, 423, 780</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>6727</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>98, 130, 423, 1073</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>6670</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>98, 130, 455, 780</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>780</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>6748</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
adding more info at top_cosine dict
</commit_message>
<xml_diff>
--- a/results/ch2_permation_residue_comb.xlsx
+++ b/results/ch2_permation_residue_comb.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>130, 780</t>
+          <t>130, 455, 780</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -471,14 +471,14 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>3631</t>
+          <t>5269</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>455</t>
+          <t>1073, 1105</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -486,19 +486,19 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>455</t>
+          <t>1105</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>3666</t>
+          <t>5131</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1073, 1105</t>
+          <t>130, 1073, 1105</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -511,34 +511,34 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>5131</t>
+          <t>5399</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>130, 1073</t>
+          <t>423, 748, 780, 1073</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>780, 780</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>4415</t>
+          <t>5677, 5887</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>780, 1073, 1105</t>
+          <t>423, 1105, 1105</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -551,34 +551,34 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>4994</t>
+          <t>5331</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>130, 455, 780</t>
+          <t>423, 1073, 1105</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>130, 130</t>
+          <t>1105</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>5269, 6424</t>
+          <t>5433</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>130, 1073, 1105</t>
+          <t>98, 130, 748, 1073</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -586,232 +586,12 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1105</t>
+          <t>130</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>5399</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>423, 748, 780, 1073</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>2</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>780, 780</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>5677, 5887</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>423, 1105, 1105</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>1</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>1105</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>5331</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>423, 1073, 1105</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>1</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>1105</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>5433</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>98, 130, 748, 780, 1073</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>1</v>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>6016</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>98, 130, 748, 1073</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>2</v>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>130, 130</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>5582, 6488</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>423, 748, 780, 1073, SF</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>1</v>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>780</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>6202</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>130, 423, 748, 1073</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>1</v>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>6561</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>130, 780, 1073, 1105</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>1</v>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>1105</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>6359</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>98, 130, 130, 423, 780</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>1</v>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>6727</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>98, 130, 423, 1073</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>1</v>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>6670</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>98, 130, 455, 780</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>1</v>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>780</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>6748</t>
+          <t>5582</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
adding more info at top_cosine dict for all frames
</commit_message>
<xml_diff>
--- a/results/ch2_permation_residue_comb.xlsx
+++ b/results/ch2_permation_residue_comb.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>130, 455, 780</t>
+          <t>130, 780</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -471,14 +471,14 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>5269</t>
+          <t>3631</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1073, 1105</t>
+          <t>455</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -486,19 +486,19 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>1105</t>
+          <t>455</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>5131</t>
+          <t>3666</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>130, 1073, 1105</t>
+          <t>1073, 1105</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -511,34 +511,34 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>5399</t>
+          <t>5131</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>423, 748, 780, 1073</t>
+          <t>130, 1073</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>780, 780</t>
+          <t>130</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>5677, 5887</t>
+          <t>4415</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>423, 1105, 1105</t>
+          <t>780, 1073, 1105</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -551,47 +551,267 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>5331</t>
+          <t>4994</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>423, 1073, 1105</t>
+          <t>130, 455, 780</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1105</t>
+          <t>130, 130</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>5433</t>
+          <t>5269, 6424</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>130, 1073, 1105</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>1105</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>5399</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>423, 748, 780, 1073</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>780, 780</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>5677, 5887</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>423, 1105, 1105</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>1105</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>5331</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>423, 1073, 1105</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1105</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>5433</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>98, 130, 748, 780, 1073</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>6016</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
           <t>98, 130, 748, 1073</t>
         </is>
       </c>
-      <c r="B8" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" t="inlineStr">
+      <c r="B13" t="n">
+        <v>2</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>130, 130</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>5582, 6488</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>423, 748, 780, 1073, SF</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>780</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>6202</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>130, 423, 748, 1073</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" t="inlineStr">
         <is>
           <t>130</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>5582</t>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>6561</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>130, 780, 1073, 1105</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>1105</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>6359</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>98, 130, 130, 423, 780</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>6727</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>98, 130, 423, 1073</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>6670</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>98, 130, 455, 780</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>780</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>6748</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
calculate min atom distances
</commit_message>
<xml_diff>
--- a/results/ch2_permation_residue_comb.xlsx
+++ b/results/ch2_permation_residue_comb.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,7 +478,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>455</t>
+          <t>780</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -486,7 +486,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>455</t>
+          <t>780</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -498,27 +498,27 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1073, 1105</t>
+          <t>130, 1073</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1105</t>
+          <t>130, 130</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>5131</t>
+          <t>5131, 4415</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>130, 1073</t>
+          <t>780, 1073, 1105</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -526,79 +526,79 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>1105</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>4415</t>
+          <t>4994</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>780, 1073, 1105</t>
+          <t>130, 455, 780</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1105</t>
+          <t>130, 130</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>4994</t>
+          <t>5269, 6424</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>130, 455, 780</t>
+          <t>455, 1073, 1105</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>130, 130</t>
+          <t>1105</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>5269, 6424</t>
+          <t>5399</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>130, 1073, 1105</t>
+          <t>423, 748, 780, 1073</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1105</t>
+          <t>780, 780</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>5399</t>
+          <t>5677, 5887</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>423, 748, 780, 1073</t>
+          <t>423, 1073, 1105</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -606,19 +606,19 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>780, 780</t>
+          <t>1105, 1105</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>5677, 5887</t>
+          <t>5331, 5433</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>423, 1105, 1105</t>
+          <t>98, 130, 455, 748, 1073</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -626,19 +626,19 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1105</t>
+          <t>130</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>5331</t>
+          <t>6016</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>423, 1073, 1105</t>
+          <t>98, 130, 748, 1073</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -646,19 +646,19 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1105</t>
+          <t>130</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>5433</t>
+          <t>5582</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>98, 130, 748, 780, 1073</t>
+          <t>130, 423, 748, 1073, SF</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -671,34 +671,34 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>6016</t>
+          <t>6202</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>98, 130, 748, 1073</t>
+          <t>98, 130, 780, 1073</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>130, 130</t>
+          <t>130</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>5582, 6488</t>
+          <t>6488</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>423, 748, 780, 1073, SF</t>
+          <t>130, 423, 780, 1073</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -706,19 +706,19 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>780</t>
+          <t>130</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>6202</t>
+          <t>6561</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>130, 423, 748, 1073</t>
+          <t>130, 780, 780, 1073</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -726,19 +726,19 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>780</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>6561</t>
+          <t>6359</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>130, 780, 1073, 1105</t>
+          <t>98, 98, 130, 455, 780</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -746,19 +746,19 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1105</t>
+          <t>130</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>6359</t>
+          <t>6727</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>98, 130, 130, 423, 780</t>
+          <t>98, 130, 423, 1073</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -771,14 +771,14 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>6727</t>
+          <t>6670</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>98, 130, 423, 1073</t>
+          <t>98, 98, 455, 780</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -786,30 +786,10 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>780</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
-        <is>
-          <t>6670</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>98, 130, 455, 780</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>1</v>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>780</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
         <is>
           <t>6748</t>
         </is>

</xml_diff>

<commit_message>
df for forces at permeation
</commit_message>
<xml_diff>
--- a/results/ch2_permation_residue_comb.xlsx
+++ b/results/ch2_permation_residue_comb.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>130, 780</t>
+          <t>130, 455, 780</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -471,14 +471,14 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>3631</t>
+          <t>5269</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>780</t>
+          <t>130, 1073</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -486,59 +486,59 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>780</t>
+          <t>130</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>3666</t>
+          <t>5131</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>130, 1073</t>
+          <t>455, 1073, 1105</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>130, 130</t>
+          <t>1105</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>5131, 4415</t>
+          <t>5399</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>780, 1073, 1105</t>
+          <t>423, 748, 780, 1073</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1105</t>
+          <t>780, 780</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>4994</t>
+          <t>5677, 5887</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>130, 455, 780</t>
+          <t>423, 1073, 1105</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -546,19 +546,19 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>130, 130</t>
+          <t>1105, 1105</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>5269, 6424</t>
+          <t>5331, 5433</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>455, 1073, 1105</t>
+          <t>98, 130, 748, 1073</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -566,232 +566,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1105</t>
+          <t>130</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>5399</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>423, 748, 780, 1073</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>2</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>780, 780</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>5677, 5887</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>423, 1073, 1105</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>2</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>1105, 1105</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>5331, 5433</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>98, 130, 455, 748, 1073</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>1</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>6016</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>98, 130, 748, 1073</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>1</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
           <t>5582</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>130, 423, 748, 1073, SF</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>1</v>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>6202</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>98, 130, 780, 1073</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>1</v>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>6488</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>130, 423, 780, 1073</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>1</v>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>6561</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>130, 780, 780, 1073</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>1</v>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>780</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>6359</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>98, 98, 130, 455, 780</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>1</v>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>6727</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>98, 130, 423, 1073</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>1</v>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>6670</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>98, 98, 455, 780</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>1</v>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>780</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>6748</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
df for forces at permeation - 3000:6799
</commit_message>
<xml_diff>
--- a/results/ch2_permation_residue_comb.xlsx
+++ b/results/ch2_permation_residue_comb.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>130, 455, 780</t>
+          <t>130, 780</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -471,14 +471,14 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>5269</t>
+          <t>3631</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>130, 1073</t>
+          <t>780</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -486,59 +486,59 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>780</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>5131</t>
+          <t>3666</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>455, 1073, 1105</t>
+          <t>130, 1073</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1105</t>
+          <t>130, 130</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>5399</t>
+          <t>5131, 4415</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>423, 748, 780, 1073</t>
+          <t>780, 1073, 1105</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>780, 780</t>
+          <t>1105</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>5677, 5887</t>
+          <t>4994</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>423, 1073, 1105</t>
+          <t>130, 455, 780</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -546,32 +546,252 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1105, 1105</t>
+          <t>130, 130</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>5331, 5433</t>
+          <t>5269, 6424</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>455, 1073, 1105</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>1105</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>5399</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>423, 748, 780, 1073</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>780, 780</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>5677, 5887</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>423, 1073, 1105</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>1105, 1105</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>5331, 5433</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>98, 130, 455, 748, 1073</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>6016</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
           <t>98, 130, 748, 1073</t>
         </is>
       </c>
-      <c r="B7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" t="inlineStr">
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" t="inlineStr">
         <is>
           <t>130</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>5582</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>130, 423, 748, 1073, SF</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>6202</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>98, 130, 780, 1073</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>6488</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>130, 423, 780, 1073</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>6561</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>130, 780, 780, 1073</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>780</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>6359</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>98, 98, 130, 455, 780</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>6727</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>98, 130, 423, 1073</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>6670</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>98, 98, 455, 780</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>780</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>6748</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
dipole distance in ch2
</commit_message>
<xml_diff>
--- a/results/ch2_permation_residue_comb.xlsx
+++ b/results/ch2_permation_residue_comb.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>130, 780</t>
+          <t>130, 423, 780, 1073</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -471,14 +471,14 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>3631</t>
+          <t>6562</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>780</t>
+          <t>98, 130, 423</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -486,39 +486,39 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>780</t>
+          <t>130</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>3666</t>
+          <t>6427</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>130, 1073</t>
+          <t>98, 130, 455, 1073</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>130, 130</t>
+          <t>130</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>5131, 4415</t>
+          <t>6489</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>780, 1073, 1105</t>
+          <t>98, 130, 748, 780, 1073</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -526,39 +526,39 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1105</t>
+          <t>130</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>4994</t>
+          <t>6017</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>130, 455, 780</t>
+          <t>130, 423, 748, 1073, SF</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>130, 130</t>
+          <t>130</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>5269, 6424</t>
+          <t>6202</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>455, 1073, 1105</t>
+          <t>130, 780, 780, 1073</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -566,59 +566,59 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1105</t>
+          <t>780</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>5399</t>
+          <t>6359</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>423, 748, 780, 1073</t>
+          <t>98, 98, 130, 455, 780</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>780, 780</t>
+          <t>130</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>5677, 5887</t>
+          <t>6727</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>423, 1073, 1105</t>
+          <t>98, 130, 423, 1073</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1105, 1105</t>
+          <t>130</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>5331, 5433</t>
+          <t>6670</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>98, 130, 455, 748, 1073</t>
+          <t>98, 98, 455, 780</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -626,170 +626,10 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>780</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
-        <is>
-          <t>6016</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>98, 130, 748, 1073</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>1</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>5582</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>130, 423, 748, 1073, SF</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>1</v>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>6202</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>98, 130, 780, 1073</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>1</v>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>6488</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>130, 423, 780, 1073</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>1</v>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>6561</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>130, 780, 780, 1073</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>1</v>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>780</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>6359</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>98, 98, 130, 455, 780</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>1</v>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>6727</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>98, 130, 423, 1073</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>1</v>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>6670</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>98, 98, 455, 780</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>1</v>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>780</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
         <is>
           <t>6748</t>
         </is>

</xml_diff>

<commit_message>
all 6799 frames run
</commit_message>
<xml_diff>
--- a/results/ch2_permation_residue_comb.xlsx
+++ b/results/ch2_permation_residue_comb.xlsx
@@ -458,40 +458,40 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>98, 423, 780, 1105</t>
+          <t>98, 130, 748, 1073</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>780</t>
+          <t>130, 130</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>5552</t>
+          <t>5178, 5582</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>98, 130, 748, 1073</t>
+          <t>98, 423, 780, 1105</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>130, 130</t>
+          <t>780</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>5178, 5582</t>
+          <t>5552</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
distances based on charges 6799 frames results
</commit_message>
<xml_diff>
--- a/results/ch2_permation_residue_comb.xlsx
+++ b/results/ch2_permation_residue_comb.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>98, 130, 748, 1073</t>
+          <t>130, 130, 780, 1105</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -478,7 +478,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>98, 423, 780, 1105</t>
+          <t>130, 455, 780, 780</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -518,7 +518,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>98, 130, 748, 780</t>
+          <t>130, 130, 780, 780</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -558,47 +558,47 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>130, 423, 748, 1073</t>
+          <t>455, 780, 1105, 1105</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>1105, 1105, 1105, 1105</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>5131</t>
+          <t>5131, 5331, 5433, 6562</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>98, 130, 455, 1073</t>
+          <t>130, 130, 455, 1105</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>130, 130</t>
+          <t>130, 130, 130</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>4416, 6489</t>
+          <t>4416, 6489, 6670</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>130, 423, 423, 780, 1073</t>
+          <t>455, 780, 1105, 1105, SF</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -606,7 +606,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>1105</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -618,7 +618,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>130, 455, 748, 780</t>
+          <t>130, 455, 780, 1105</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -638,27 +638,27 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>98, 748, 1073, 1105</t>
+          <t>130, 780, 1105, 1105</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1105</t>
+          <t>1105, 1105</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>5400</t>
+          <t>5400, 6359</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>423, 748, 780, 1073</t>
+          <t>455, 780, 780, 1105</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -678,27 +678,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>423, 748, 1073, 1105</t>
+          <t>455, 455, 780, 1105</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>1105, 1105</t>
+          <t>455</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>5331, 5433</t>
+          <t>5886</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>423, 455, 748, 1073</t>
+          <t>130, 130, 780, 780, 1105</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -706,19 +706,19 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>455</t>
+          <t>130</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>5886</t>
+          <t>6017</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>98, 130, 748, 780, 1073</t>
+          <t>455, 780, 780, 1105, SF</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -726,19 +726,19 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>780</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>6017</t>
+          <t>6202</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>130, 423, 748, 1073, SF</t>
+          <t>130, 130, 455</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -751,14 +751,14 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>6202</t>
+          <t>6427</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>98, 130, 423</t>
+          <t>130, 130, 130, 455, 780</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -771,14 +771,14 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>6427</t>
+          <t>6727</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>130, 423, 780, 1073</t>
+          <t>130, 455, 780, SF</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -786,90 +786,10 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>780</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
-        <is>
-          <t>6562</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>130, 780, 780, 1073</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>1</v>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>780</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>6359</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>98, 98, 130, 455, 780</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>1</v>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>6727</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>98, 130, 423, 1073</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>1</v>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>6670</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>98, 98, 455, 780</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>1</v>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>780</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
         <is>
           <t>6748</t>
         </is>

</xml_diff>

<commit_message>
distances based on charges - correct positions of residues in every frame
</commit_message>
<xml_diff>
--- a/results/ch2_permation_residue_comb.xlsx
+++ b/results/ch2_permation_residue_comb.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,27 +458,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>130, 130, 780, 1105</t>
+          <t>98, 130, 748, 1073</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>130, 130</t>
+          <t>130, 130, 130</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>5178, 5582</t>
+          <t>5178, 5400, 5582</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>130, 455, 780, 780</t>
+          <t>98, 455, 780, 1105</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -518,7 +518,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>130, 130, 780, 780</t>
+          <t>98, 130, 748, 780</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -538,7 +538,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>130, 780, 1105</t>
+          <t>98, 780, 1105</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -558,47 +558,47 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>455, 780, 1105, 1105</t>
+          <t>130, 455, 748, 1073</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1105, 1105, 1105, 1105</t>
+          <t>130</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>5131, 5331, 5433, 6562</t>
+          <t>5131</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>130, 130, 455, 1105</t>
+          <t>98, 130, 455, 1073</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>130, 130, 130</t>
+          <t>130, 130</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>4416, 6489, 6670</t>
+          <t>4416, 6489</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>455, 780, 1105, 1105, SF</t>
+          <t>130, 423, 1073, SF, SF</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -606,7 +606,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1105</t>
+          <t>130</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -618,7 +618,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>130, 455, 780, 1105</t>
+          <t>130, 455, 748, 780</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -638,47 +638,47 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>130, 780, 1105, 1105</t>
+          <t>423, 748, 780, 1073</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1105, 1105</t>
+          <t>780</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>5400, 6359</t>
+          <t>5677</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>455, 780, 780, 1105</t>
+          <t>423, 748, 1073, 1105</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>780</t>
+          <t>1105, 1105</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>5677</t>
+          <t>5331, 5433</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>455, 455, 780, 1105</t>
+          <t>130, 423, 748, 1073</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -686,7 +686,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>455</t>
+          <t>130</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -698,7 +698,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>130, 130, 780, 780, 1105</t>
+          <t>98, 130, 748, 780, 1073</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -718,7 +718,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>455, 780, 780, 1105, SF</t>
+          <t>130, 423, 748, 1073, SF</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -726,7 +726,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>780</t>
+          <t>130</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -738,7 +738,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>130, 130, 455</t>
+          <t>98, 130, 423</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -758,7 +758,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>130, 130, 130, 455, 780</t>
+          <t>130, 455, 780, 1073</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -771,14 +771,14 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>6727</t>
+          <t>6562</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>130, 455, 780, SF</t>
+          <t>98, 780, 780, 1105</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -790,6 +790,66 @@
         </is>
       </c>
       <c r="D18" t="inlineStr">
+        <is>
+          <t>6359</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>98, 130, 130, 455, 780</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>6727</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>130, 130, 423, 1073</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>6670</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>98, 98, 455, 455</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>455</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
         <is>
           <t>6748</t>
         </is>

</xml_diff>

<commit_message>
close contact residues within 6A added
</commit_message>
<xml_diff>
--- a/results/ch2_permation_residue_comb.xlsx
+++ b/results/ch2_permation_residue_comb.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,7 +471,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>5178, 5400, 5582</t>
+          <t>5178, 5582, 6488</t>
         </is>
       </c>
     </row>
@@ -578,27 +578,27 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>98, 130, 455, 1073</t>
+          <t>98, 130, 1073, SF</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>130, 130</t>
+          <t>130</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>4416, 6489</t>
+          <t>4415</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>130, 423, 1073, SF, SF</t>
+          <t>423, 1073, 1105, SF, SF</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -606,12 +606,12 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>1105</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>4995</t>
+          <t>4994</t>
         </is>
       </c>
     </row>
@@ -638,7 +638,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>423, 748, 780, 1073</t>
+          <t>130, 748, 1073, 1105</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -646,59 +646,59 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>780</t>
+          <t>1105</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>5677</t>
+          <t>5399</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>423, 748, 1073, 1105</t>
+          <t>423, 748, 780, 1073</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1105, 1105</t>
+          <t>780</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>5331, 5433</t>
+          <t>5677</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>130, 423, 748, 1073</t>
+          <t>423, 748, 1073, 1105</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>1105, 1105</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>5886</t>
+          <t>5331, 5433</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>98, 130, 748, 780, 1073</t>
+          <t>130, 423, 748, 1073</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -711,14 +711,14 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>6017</t>
+          <t>5886</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>130, 423, 748, 1073, SF</t>
+          <t>98, 130, 455, 748, 1073</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -731,14 +731,14 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>6202</t>
+          <t>6016</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>98, 130, 423</t>
+          <t>130, 423, 748, 1073, SF</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -751,14 +751,14 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>6427</t>
+          <t>6202</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>130, 455, 780, 1073</t>
+          <t>130, 130, 423</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -771,14 +771,14 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>6562</t>
+          <t>6426</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>98, 780, 780, 1105</t>
+          <t>130, 455, 780, 1105</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -786,19 +786,19 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>780</t>
+          <t>130</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>6359</t>
+          <t>6561</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>98, 130, 130, 455, 780</t>
+          <t>98, 780, 780, 1105</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -806,19 +806,19 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>780</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>6727</t>
+          <t>6359</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>130, 130, 423, 1073</t>
+          <t>98, 130, 130, 455, 780</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -831,25 +831,45 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>6670</t>
+          <t>6727</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
+          <t>130, 130, 423, 1073</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>6670</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
           <t>98, 98, 455, 455</t>
         </is>
       </c>
-      <c r="B21" t="n">
-        <v>1</v>
-      </c>
-      <c r="C21" t="inlineStr">
+      <c r="B22" t="n">
+        <v>1</v>
+      </c>
+      <c r="C22" t="inlineStr">
         <is>
           <t>455</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
+      <c r="D22" t="inlineStr">
         <is>
           <t>6748</t>
         </is>

</xml_diff>

<commit_message>
json that handles the closest_residues_comb - draft version
</commit_message>
<xml_diff>
--- a/results/ch2_permation_residue_comb.xlsx
+++ b/results/ch2_permation_residue_comb.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,27 +458,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>98, 130, 748, 1073</t>
+          <t>98, 130, 130, 455, 780</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>130, 130, 130</t>
+          <t>130</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>5178, 5582, 6488</t>
+          <t>6727</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>98, 455, 780, 1105</t>
+          <t>130, 455, 780, 1105</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -486,19 +486,19 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>780</t>
+          <t>130</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>5552</t>
+          <t>6561</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>130, 780, 780</t>
+          <t>130, 130, 423, 1073</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -511,14 +511,14 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>3171</t>
+          <t>6670</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>98, 130, 748, 780</t>
+          <t>98, 98, 455, 455</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -526,350 +526,10 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>455</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
-        <is>
-          <t>3631</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>98, 780, 1105</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>780</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>3666</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>130, 455, 748, 1073</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>5131</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>98, 130, 1073, SF</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>4415</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>423, 1073, 1105, SF, SF</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>1105</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>4994</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>130, 455, 748, 780</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>1</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>5269</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>130, 748, 1073, 1105</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>1</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>1105</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>5399</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>423, 748, 780, 1073</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>1</v>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>780</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>5677</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>423, 748, 1073, 1105</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>2</v>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>1105, 1105</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>5331, 5433</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>130, 423, 748, 1073</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>1</v>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>5886</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>98, 130, 455, 748, 1073</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>1</v>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>6016</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>130, 423, 748, 1073, SF</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>1</v>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>6202</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>130, 130, 423</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>1</v>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>6426</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>130, 455, 780, 1105</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>1</v>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>6561</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>98, 780, 780, 1105</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>1</v>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>780</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>6359</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>98, 130, 130, 455, 780</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>1</v>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>6727</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>130, 130, 423, 1073</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>1</v>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>6670</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>98, 98, 455, 455</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>1</v>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>455</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
         <is>
           <t>6748</t>
         </is>

</xml_diff>

<commit_message>
json that handles the closest_residues_comb - draft version: 6799 frames
</commit_message>
<xml_diff>
--- a/results/ch2_permation_residue_comb.xlsx
+++ b/results/ch2_permation_residue_comb.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,27 +458,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>98, 130, 130, 455, 780</t>
+          <t>98, 130, 748, 1073</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>130, 130, 130</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>6727</t>
+          <t>5178, 5582, 6488</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>130, 455, 780, 1105</t>
+          <t>98, 455, 780, 1105</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -486,19 +486,19 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>780</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>6561</t>
+          <t>5552</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>130, 130, 423, 1073</t>
+          <t>130, 780, 780</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -511,25 +511,365 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>6670</t>
+          <t>3171</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>98, 130, 748, 780</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>3631</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>98, 780, 1105</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>780</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>3666</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>130, 455, 748, 1073</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>5131</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>98, 130, 1073, SF</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>4415</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>423, 1073, 1105, SF, SF</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>1105</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>4994</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>130, 455, 748, 780</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>5269</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>130, 748, 1073, 1105</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1105</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>5399</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>423, 748, 780, 1073</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>780</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>5677</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>423, 748, 1073, 1105</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>2</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>1105, 1105</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>5331, 5433</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>130, 423, 748, 1073</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>5886</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>98, 130, 455, 748, 1073</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>6016</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>130, 423, 748, 1073, SF</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>6202</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>130, 130, 423</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>6426</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>130, 455, 780, 1105</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>6561</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>98, 780, 780, 1105</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>780</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>6359</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>98, 130, 130, 455, 780</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>6727</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>130, 130, 423, 1073</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>6670</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
           <t>98, 98, 455, 455</t>
         </is>
       </c>
-      <c r="B5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" t="inlineStr">
+      <c r="B22" t="n">
+        <v>1</v>
+      </c>
+      <c r="C22" t="inlineStr">
         <is>
           <t>455</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="D22" t="inlineStr">
         <is>
           <t>6748</t>
         </is>

</xml_diff>

<commit_message>
creation of PermeationAnalyzer class
</commit_message>
<xml_diff>
--- a/results/ch2_permation_residue_comb.xlsx
+++ b/results/ch2_permation_residue_comb.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,27 +458,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>98, 130, 748, 1073</t>
+          <t>98, 130, 130, 455, 780</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>130, 130, 130</t>
+          <t>130</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>5178, 5582, 6488</t>
+          <t>6727</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>98, 455, 780, 1105</t>
+          <t>130, 455, 780, 1105</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -486,19 +486,19 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>780</t>
+          <t>130</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>5552</t>
+          <t>6561</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>130, 780, 780</t>
+          <t>130, 130, 423, 1073</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -511,14 +511,14 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>3171</t>
+          <t>6670</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>98, 130, 748, 780</t>
+          <t>98, 98, 455, 455</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -526,350 +526,10 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>455</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
-        <is>
-          <t>3631</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>98, 780, 1105</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>780</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>3666</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>130, 455, 748, 1073</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>5131</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>98, 130, 1073, SF</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>4415</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>423, 1073, 1105, SF, SF</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>1105</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>4994</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>130, 455, 748, 780</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>1</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>5269</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>130, 748, 1073, 1105</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>1</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>1105</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>5399</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>423, 748, 780, 1073</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>1</v>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>780</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>5677</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>423, 748, 1073, 1105</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>2</v>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>1105, 1105</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>5331, 5433</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>130, 423, 748, 1073</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>1</v>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>5886</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>98, 130, 455, 748, 1073</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>1</v>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>6016</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>130, 423, 748, 1073, SF</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>1</v>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>6202</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>130, 130, 423</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>1</v>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>6426</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>130, 455, 780, 1105</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>1</v>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>6561</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>98, 780, 780, 1105</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>1</v>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>780</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>6359</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>98, 130, 130, 455, 780</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>1</v>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>6727</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>130, 130, 423, 1073</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>1</v>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>6670</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>98, 98, 455, 455</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>1</v>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>455</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
         <is>
           <t>6748</t>
         </is>

</xml_diff>

<commit_message>
creation of PermeationAnalyzer class: 6799 frames
</commit_message>
<xml_diff>
--- a/results/ch2_permation_residue_comb.xlsx
+++ b/results/ch2_permation_residue_comb.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,27 +458,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>98, 130, 130, 455, 780</t>
+          <t>98, 130, 748, 1073</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>130, 130, 130</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>6727</t>
+          <t>5178, 5582, 6488</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>130, 455, 780, 1105</t>
+          <t>98, 455, 780, 1105</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -486,19 +486,19 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>780</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>6561</t>
+          <t>5552</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>130, 130, 423, 1073</t>
+          <t>130, 780, 780</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -511,25 +511,365 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>6670</t>
+          <t>3171</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>98, 130, 748, 780</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>3631</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>98, 780, 1105</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>780</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>3666</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>130, 455, 748, 1073</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>5131</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>98, 130, 1073, SF</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>4415</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>423, 1073, 1105, SF, SF</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>1105</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>4994</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>130, 455, 748, 780</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>5269</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>130, 748, 1073, 1105</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1105</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>5399</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>423, 748, 780, 1073</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>780</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>5677</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>423, 748, 1073, 1105</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>2</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>1105, 1105</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>5331, 5433</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>130, 423, 748, 1073</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>5886</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>98, 130, 455, 748, 1073</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>6016</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>130, 423, 748, 1073, SF</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>6202</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>130, 130, 423</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>6426</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>130, 455, 780, 1105</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>6561</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>98, 780, 780, 1105</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>780</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>6359</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>98, 130, 130, 455, 780</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>6727</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>130, 130, 423, 1073</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>6670</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
           <t>98, 98, 455, 455</t>
         </is>
       </c>
-      <c r="B5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" t="inlineStr">
+      <c r="B22" t="n">
+        <v>1</v>
+      </c>
+      <c r="C22" t="inlineStr">
         <is>
           <t>455</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="D22" t="inlineStr">
         <is>
           <t>6748</t>
         </is>

</xml_diff>

<commit_message>
finding pattern in frames original pdb numbering added
</commit_message>
<xml_diff>
--- a/results/ch2_permation_residue_comb.xlsx
+++ b/results/ch2_permation_residue_comb.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,27 +458,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>98, 130, 130, 455, 780</t>
+          <t>98, 130, 748, 1073</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>130, 130, 130</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>6727</t>
+          <t>5178, 5582, 6488</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>130, 455, 780, 1105</t>
+          <t>98, 455, 780, 1105</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -486,19 +486,19 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>780</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>6561</t>
+          <t>5552</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>130, 130, 423, 1073</t>
+          <t>130, 780, 780</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -511,25 +511,365 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>6670</t>
+          <t>3171</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>98, 130, 748, 780</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>3631</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>98, 780, 1105</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>780</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>3666</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>130, 455, 748, 1073</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>5131</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>98, 130, 1073, SF</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>4415</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>423, 1073, 1105, SF, SF</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>1105</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>4994</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>130, 455, 748, 780</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>5269</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>130, 748, 1073, 1105</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1105</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>5399</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>423, 748, 780, 1073</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>780</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>5677</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>423, 748, 1073, 1105</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>2</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>1105, 1105</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>5331, 5433</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>130, 423, 748, 1073</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>5886</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>98, 130, 455, 748, 1073</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>6016</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>130, 423, 748, 1073, SF</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>6202</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>130, 130, 423</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>6426</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>130, 455, 780, 1105</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>6561</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>98, 780, 780, 1105</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>780</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>6359</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>98, 130, 130, 455, 780</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>6727</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>130, 130, 423, 1073</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>6670</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
           <t>98, 98, 455, 455</t>
         </is>
       </c>
-      <c r="B5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" t="inlineStr">
+      <c r="B22" t="n">
+        <v>1</v>
+      </c>
+      <c r="C22" t="inlineStr">
         <is>
           <t>455</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="D22" t="inlineStr">
         <is>
           <t>6748</t>
         </is>

</xml_diff>